<commit_message>
fixed market trend and added short-term watchlist
</commit_message>
<xml_diff>
--- a/updater/source.xlsx
+++ b/updater/source.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MyBroKe\updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704D6548-2833-4DD9-A05C-11ACCEE89937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ED33EC-55C0-4F8A-A63E-2B5A83FE0CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18480" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18470" windowHeight="12220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AssetSector" sheetId="1" r:id="rId1"/>
     <sheet name="AssetCountry" sheetId="2" r:id="rId2"/>
     <sheet name="FundTransferHistory" sheetId="3" r:id="rId3"/>
+    <sheet name="STWatchlist" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">AssetCountry!$1:$124</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="123">
   <si>
     <t>Datadate</t>
   </si>
@@ -335,6 +336,78 @@
   </si>
   <si>
     <t>EntryDatetime</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Horizon</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Show</t>
+  </si>
+  <si>
+    <t>Entry Datetime</t>
+  </si>
+  <si>
+    <t>VCLT</t>
+  </si>
+  <si>
+    <t>Rising interest rate generally enhance bond performance</t>
+  </si>
+  <si>
+    <t>TLT</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>US long-term corp bond</t>
+  </si>
+  <si>
+    <t>US long-term gov bond</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>Short-term</t>
+  </si>
+  <si>
+    <t>XLF</t>
+  </si>
+  <si>
+    <t>Financial sector tend to perform better in rising interest rate environment</t>
+  </si>
+  <si>
+    <t>US financial sector index</t>
+  </si>
+  <si>
+    <t>Look Up Symbol</t>
+  </si>
+  <si>
+    <t>Medium-term</t>
+  </si>
+  <si>
+    <t>Private equity</t>
+  </si>
+  <si>
+    <t>Pension fund increase exposure to PE</t>
+  </si>
+  <si>
+    <t>Pension fund increase exposure to ESG</t>
+  </si>
+  <si>
+    <t>ESG</t>
   </si>
 </sst>
 </file>
@@ -6241,8 +6314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24FBA74-073E-46F2-A677-303D1306A835}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="H20:I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6325,4 +6398,230 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940DB676-0691-4D6D-967D-ED592843676B}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="str">
+        <f>A2&amp;"-"&amp;B2</f>
+        <v>VCLT-USD</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="14">
+        <v>44628.725694444445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C6" si="0">A3&amp;"-"&amp;B3</f>
+        <v>TLT-USD</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="14">
+        <v>44628.725694444445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>XLF-USD</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="14">
+        <v>44628.725694444445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="14">
+        <v>44628.725694444445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="14">
+        <v>44628.725694444445</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add other account info
</commit_message>
<xml_diff>
--- a/updater/source.xlsx
+++ b/updater/source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MyBroKe\updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5DEE23-9525-499B-86DA-EAE8651B4A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE834B4E-1FBB-4535-96CA-E32E19474EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18470" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18470" windowHeight="12220" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AssetSector" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="FundTransferHistory" sheetId="3" r:id="rId3"/>
     <sheet name="STWatchlist" sheetId="4" r:id="rId4"/>
     <sheet name="AssetChar" sheetId="5" r:id="rId5"/>
+    <sheet name="FundTransferHistory2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">AssetChar!$A$1:$K$1</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="167">
   <si>
     <t>Datadate</t>
   </si>
@@ -520,12 +521,36 @@
   </si>
   <si>
     <t>Withdrawal</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>LIRA Ke</t>
+  </si>
+  <si>
+    <t>TFSA Tong</t>
+  </si>
+  <si>
+    <t>Account Value</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Intrim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -975,7 +1000,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1018,8 +1043,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1050,8 +1076,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1079,6 +1106,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -7522,8 +7550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24FBA74-073E-46F2-A677-303D1306A835}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8855,4 +8883,194 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19D8F81-04A5-4D1F-90EE-02C5BAFD5B03}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G3:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>44637</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="18">
+        <v>139895.32999999999</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12">
+        <v>44784.838888888888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>44784</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="18">
+        <v>134823</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
+        <v>44784.838888888888</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>44586</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="18">
+        <v>50000</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
+        <v>44784.838888888888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>44616</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="18">
+        <v>15000</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12">
+        <v>44784.838888888888</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>44742</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="18">
+        <v>20000</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12">
+        <v>44784.838888888888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>44784</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="18">
+        <v>85406</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12">
+        <v>44784.838888888888</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{DB11C3E3-B056-422F-AAFC-F6CF592652EC}">
+      <formula1>"LIRA Ke, RRSP Ke, RRSP Tong, TFSA Ke, TFSA Tong"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
To include multiple accounts
</commit_message>
<xml_diff>
--- a/updater/source.xlsx
+++ b/updater/source.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\MyBroKe\updater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE834B4E-1FBB-4535-96CA-E32E19474EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6B7050-B292-4C36-99F9-9CD8641B3B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18470" windowHeight="12220" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="18240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AssetSector" sheetId="1" r:id="rId1"/>
     <sheet name="AssetCountry" sheetId="2" r:id="rId2"/>
-    <sheet name="FundTransferHistory" sheetId="3" r:id="rId3"/>
-    <sheet name="STWatchlist" sheetId="4" r:id="rId4"/>
-    <sheet name="AssetChar" sheetId="5" r:id="rId5"/>
-    <sheet name="FundTransferHistory2" sheetId="6" r:id="rId6"/>
+    <sheet name="STWatchlist" sheetId="4" r:id="rId3"/>
+    <sheet name="AssetChar" sheetId="5" r:id="rId4"/>
+    <sheet name="MyBrokerAccounts" sheetId="7" r:id="rId5"/>
+    <sheet name="FundTransferHistory" sheetId="3" r:id="rId6"/>
+    <sheet name="FundTransferHistoryOA" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">AssetChar!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AssetChar!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">AssetCountry!$A$1:$G$140</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AssetSector!$A$1:$G$116</definedName>
   </definedNames>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="185">
   <si>
     <t>Datadate</t>
   </si>
@@ -523,15 +524,6 @@
     <t>Withdrawal</t>
   </si>
   <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>LIRA Ke</t>
-  </si>
-  <si>
-    <t>TFSA Tong</t>
-  </si>
-  <si>
     <t>Account Value</t>
   </si>
   <si>
@@ -542,6 +534,69 @@
   </si>
   <si>
     <t>Intrim</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>U1989090</t>
+  </si>
+  <si>
+    <t>U10048362</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Broker</t>
+  </si>
+  <si>
+    <t>Sort Order</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Effective Date</t>
+  </si>
+  <si>
+    <t>Ke</t>
+  </si>
+  <si>
+    <t>59416078</t>
+  </si>
+  <si>
+    <t>67130182</t>
+  </si>
+  <si>
+    <t>CIBC</t>
+  </si>
+  <si>
+    <t>IB Canada</t>
+  </si>
+  <si>
+    <t>TFSA</t>
+  </si>
+  <si>
+    <t>RRSP</t>
+  </si>
+  <si>
+    <t>TFSA Saving</t>
+  </si>
+  <si>
+    <t>LIRA</t>
+  </si>
+  <si>
+    <t>60513191</t>
+  </si>
+  <si>
+    <t>67130181</t>
+  </si>
+  <si>
+    <t>Tong</t>
+  </si>
+  <si>
+    <t>Alias</t>
   </si>
 </sst>
 </file>
@@ -551,7 +606,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +744,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1045,7 +1106,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,6 +1138,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1439,18 +1501,18 @@
       <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44074</v>
       </c>
@@ -1496,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44074</v>
       </c>
@@ -1519,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44074</v>
       </c>
@@ -1542,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44074</v>
       </c>
@@ -1565,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44074</v>
       </c>
@@ -1588,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44074</v>
       </c>
@@ -1611,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44074</v>
       </c>
@@ -1634,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44074</v>
       </c>
@@ -1657,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44074</v>
       </c>
@@ -1680,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44074</v>
       </c>
@@ -1703,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44074</v>
       </c>
@@ -1726,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44074</v>
       </c>
@@ -1749,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44074</v>
       </c>
@@ -1772,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44074</v>
       </c>
@@ -1795,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44074</v>
       </c>
@@ -1818,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44074</v>
       </c>
@@ -1841,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44074</v>
       </c>
@@ -1864,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44074</v>
       </c>
@@ -1887,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44074</v>
       </c>
@@ -1910,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44074</v>
       </c>
@@ -1933,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44074</v>
       </c>
@@ -1956,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44074</v>
       </c>
@@ -1979,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44104</v>
       </c>
@@ -2002,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44104</v>
       </c>
@@ -2025,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44104</v>
       </c>
@@ -2048,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44104</v>
       </c>
@@ -2071,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44104</v>
       </c>
@@ -2094,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44104</v>
       </c>
@@ -2117,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44104</v>
       </c>
@@ -2140,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44104</v>
       </c>
@@ -2163,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44104</v>
       </c>
@@ -2186,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44104</v>
       </c>
@@ -2209,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44104</v>
       </c>
@@ -2232,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44104</v>
       </c>
@@ -2255,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44074</v>
       </c>
@@ -2278,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44074</v>
       </c>
@@ -2301,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44074</v>
       </c>
@@ -2324,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44074</v>
       </c>
@@ -2347,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44074</v>
       </c>
@@ -2370,7 +2432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44074</v>
       </c>
@@ -2393,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44074</v>
       </c>
@@ -2416,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44074</v>
       </c>
@@ -2439,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44074</v>
       </c>
@@ -2462,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44105</v>
       </c>
@@ -2485,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44105</v>
       </c>
@@ -2508,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44105</v>
       </c>
@@ -2531,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44105</v>
       </c>
@@ -2554,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44627</v>
       </c>
@@ -2577,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44627</v>
       </c>
@@ -2600,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44627</v>
       </c>
@@ -2623,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44627</v>
       </c>
@@ -2646,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44627</v>
       </c>
@@ -2669,7 +2731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44627</v>
       </c>
@@ -2692,7 +2754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44627</v>
       </c>
@@ -2715,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44627</v>
       </c>
@@ -2738,7 +2800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44627</v>
       </c>
@@ -2761,7 +2823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44627</v>
       </c>
@@ -2784,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44627</v>
       </c>
@@ -2807,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44627</v>
       </c>
@@ -2830,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44627</v>
       </c>
@@ -2853,7 +2915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44627</v>
       </c>
@@ -2876,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44627</v>
       </c>
@@ -2899,7 +2961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44627</v>
       </c>
@@ -2922,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44627</v>
       </c>
@@ -2945,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44627</v>
       </c>
@@ -2968,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44627</v>
       </c>
@@ -2991,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44627</v>
       </c>
@@ -3014,7 +3076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44627</v>
       </c>
@@ -3037,7 +3099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44627</v>
       </c>
@@ -3060,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44627</v>
       </c>
@@ -3083,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44627</v>
       </c>
@@ -3106,7 +3168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44627</v>
       </c>
@@ -3129,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44627</v>
       </c>
@@ -3152,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44627</v>
       </c>
@@ -3175,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44627</v>
       </c>
@@ -3198,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44627</v>
       </c>
@@ -3221,7 +3283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44627</v>
       </c>
@@ -3244,7 +3306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44627</v>
       </c>
@@ -3267,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44627</v>
       </c>
@@ -3290,7 +3352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44627</v>
       </c>
@@ -3313,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44627</v>
       </c>
@@ -3336,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44627</v>
       </c>
@@ -3359,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44627</v>
       </c>
@@ -3382,7 +3444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44627</v>
       </c>
@@ -3405,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44627</v>
       </c>
@@ -3428,7 +3490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44627</v>
       </c>
@@ -3451,7 +3513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44627</v>
       </c>
@@ -3474,7 +3536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44627</v>
       </c>
@@ -3497,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44627</v>
       </c>
@@ -3520,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44627</v>
       </c>
@@ -3543,7 +3605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44627</v>
       </c>
@@ -3566,7 +3628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44627</v>
       </c>
@@ -3589,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44627</v>
       </c>
@@ -3612,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44627</v>
       </c>
@@ -3635,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44628</v>
       </c>
@@ -3659,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44628</v>
       </c>
@@ -3682,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44628</v>
       </c>
@@ -3705,7 +3767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44628</v>
       </c>
@@ -3728,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44628</v>
       </c>
@@ -3751,7 +3813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44628</v>
       </c>
@@ -3774,7 +3836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44628</v>
       </c>
@@ -3797,7 +3859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44628</v>
       </c>
@@ -3820,7 +3882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44628</v>
       </c>
@@ -3843,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44628</v>
       </c>
@@ -3866,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44628</v>
       </c>
@@ -3889,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44628</v>
       </c>
@@ -3912,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44628</v>
       </c>
@@ -3935,7 +3997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44628</v>
       </c>
@@ -3958,7 +4020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44628</v>
       </c>
@@ -3981,7 +4043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44628</v>
       </c>
@@ -4004,7 +4066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44628</v>
       </c>
@@ -4027,7 +4089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44628</v>
       </c>
@@ -4050,7 +4112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44628</v>
       </c>
@@ -4073,7 +4135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44628</v>
       </c>
@@ -4096,7 +4158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44628</v>
       </c>
@@ -4119,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44655</v>
       </c>
@@ -4142,7 +4204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44783</v>
       </c>
@@ -4165,7 +4227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44783</v>
       </c>
@@ -4202,18 +4264,18 @@
       <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4236,7 +4298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44627</v>
       </c>
@@ -4259,7 +4321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44627</v>
       </c>
@@ -4282,7 +4344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44627</v>
       </c>
@@ -4305,7 +4367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44074</v>
       </c>
@@ -4329,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44074</v>
       </c>
@@ -4353,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44074</v>
       </c>
@@ -4377,7 +4439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44074</v>
       </c>
@@ -4401,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44074</v>
       </c>
@@ -4425,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44074</v>
       </c>
@@ -4449,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44074</v>
       </c>
@@ -4473,7 +4535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44105</v>
       </c>
@@ -4497,7 +4559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44627</v>
       </c>
@@ -4520,7 +4582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44104</v>
       </c>
@@ -4544,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44104</v>
       </c>
@@ -4568,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44104</v>
       </c>
@@ -4592,7 +4654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44104</v>
       </c>
@@ -4616,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44104</v>
       </c>
@@ -4640,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44104</v>
       </c>
@@ -4664,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44104</v>
       </c>
@@ -4688,7 +4750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44104</v>
       </c>
@@ -4712,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44104</v>
       </c>
@@ -4736,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44104</v>
       </c>
@@ -4760,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44104</v>
       </c>
@@ -4784,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44104</v>
       </c>
@@ -4808,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44104</v>
       </c>
@@ -4832,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44627</v>
       </c>
@@ -4855,7 +4917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44628</v>
       </c>
@@ -4878,7 +4940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44074</v>
       </c>
@@ -4902,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44074</v>
       </c>
@@ -4926,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44074</v>
       </c>
@@ -4950,7 +5012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44074</v>
       </c>
@@ -4974,7 +5036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44074</v>
       </c>
@@ -4998,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44074</v>
       </c>
@@ -5022,7 +5084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44074</v>
       </c>
@@ -5046,7 +5108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44074</v>
       </c>
@@ -5070,7 +5132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44074</v>
       </c>
@@ -5094,7 +5156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44074</v>
       </c>
@@ -5118,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44074</v>
       </c>
@@ -5142,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44105</v>
       </c>
@@ -5166,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44627</v>
       </c>
@@ -5189,7 +5251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44627</v>
       </c>
@@ -5212,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44627</v>
       </c>
@@ -5235,7 +5297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44627</v>
       </c>
@@ -5258,7 +5320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44627</v>
       </c>
@@ -5281,7 +5343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44627</v>
       </c>
@@ -5304,7 +5366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44627</v>
       </c>
@@ -5327,7 +5389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44627</v>
       </c>
@@ -5350,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44627</v>
       </c>
@@ -5373,7 +5435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44627</v>
       </c>
@@ -5396,7 +5458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44627</v>
       </c>
@@ -5419,7 +5481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44627</v>
       </c>
@@ -5442,7 +5504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44627</v>
       </c>
@@ -5465,7 +5527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44627</v>
       </c>
@@ -5488,7 +5550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44627</v>
       </c>
@@ -5511,7 +5573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44627</v>
       </c>
@@ -5534,7 +5596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>44627</v>
       </c>
@@ -5557,7 +5619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44627</v>
       </c>
@@ -5580,7 +5642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44627</v>
       </c>
@@ -5603,7 +5665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44627</v>
       </c>
@@ -5626,7 +5688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44627</v>
       </c>
@@ -5649,7 +5711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44627</v>
       </c>
@@ -5672,7 +5734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44627</v>
       </c>
@@ -5695,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44627</v>
       </c>
@@ -5718,7 +5780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44627</v>
       </c>
@@ -5741,7 +5803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44627</v>
       </c>
@@ -5764,7 +5826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44627</v>
       </c>
@@ -5787,7 +5849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44627</v>
       </c>
@@ -5810,7 +5872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44627</v>
       </c>
@@ -5833,7 +5895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44627</v>
       </c>
@@ -5856,7 +5918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44627</v>
       </c>
@@ -5879,7 +5941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44627</v>
       </c>
@@ -5902,7 +5964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44627</v>
       </c>
@@ -5925,7 +5987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44628</v>
       </c>
@@ -5948,7 +6010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44628</v>
       </c>
@@ -5971,7 +6033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44628</v>
       </c>
@@ -5994,7 +6056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44628</v>
       </c>
@@ -6017,7 +6079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44628</v>
       </c>
@@ -6040,7 +6102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44628</v>
       </c>
@@ -6063,7 +6125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44628</v>
       </c>
@@ -6086,7 +6148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44628</v>
       </c>
@@ -6109,7 +6171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44628</v>
       </c>
@@ -6132,7 +6194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44628</v>
       </c>
@@ -6155,7 +6217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44628</v>
       </c>
@@ -6178,7 +6240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44627</v>
       </c>
@@ -6201,7 +6263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44627</v>
       </c>
@@ -6224,7 +6286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44627</v>
       </c>
@@ -6247,7 +6309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44627</v>
       </c>
@@ -6270,7 +6332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44627</v>
       </c>
@@ -6293,7 +6355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44627</v>
       </c>
@@ -6316,7 +6378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44105</v>
       </c>
@@ -6340,7 +6402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44627</v>
       </c>
@@ -6363,7 +6425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44627</v>
       </c>
@@ -6386,7 +6448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44105</v>
       </c>
@@ -6410,7 +6472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44628</v>
       </c>
@@ -6433,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44627</v>
       </c>
@@ -6456,7 +6518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44074</v>
       </c>
@@ -6480,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44628</v>
       </c>
@@ -6503,7 +6565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44627</v>
       </c>
@@ -6526,7 +6588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44627</v>
       </c>
@@ -6549,7 +6611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44627</v>
       </c>
@@ -6572,7 +6634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44627</v>
       </c>
@@ -6595,7 +6657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44627</v>
       </c>
@@ -6618,7 +6680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44627</v>
       </c>
@@ -6641,7 +6703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44627</v>
       </c>
@@ -6664,7 +6726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44627</v>
       </c>
@@ -6687,7 +6749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44627</v>
       </c>
@@ -6710,7 +6772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44627</v>
       </c>
@@ -6733,7 +6795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44627</v>
       </c>
@@ -6756,7 +6818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44627</v>
       </c>
@@ -6779,7 +6841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44627</v>
       </c>
@@ -6802,7 +6864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44627</v>
       </c>
@@ -6825,7 +6887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44627</v>
       </c>
@@ -6848,7 +6910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44627</v>
       </c>
@@ -6871,7 +6933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44627</v>
       </c>
@@ -6894,7 +6956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44627</v>
       </c>
@@ -6917,7 +6979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44627</v>
       </c>
@@ -6940,7 +7002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44627</v>
       </c>
@@ -6963,7 +7025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44627</v>
       </c>
@@ -6986,7 +7048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44627</v>
       </c>
@@ -7009,7 +7071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44627</v>
       </c>
@@ -7032,7 +7094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44627</v>
       </c>
@@ -7055,7 +7117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44627</v>
       </c>
@@ -7078,7 +7140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44627</v>
       </c>
@@ -7101,7 +7163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44627</v>
       </c>
@@ -7124,7 +7186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44627</v>
       </c>
@@ -7147,7 +7209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44627</v>
       </c>
@@ -7170,7 +7232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44627</v>
       </c>
@@ -7193,7 +7255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44627</v>
       </c>
@@ -7216,7 +7278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44627</v>
       </c>
@@ -7239,7 +7301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44627</v>
       </c>
@@ -7262,7 +7324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44627</v>
       </c>
@@ -7285,7 +7347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44627</v>
       </c>
@@ -7308,7 +7370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44627</v>
       </c>
@@ -7331,7 +7393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44627</v>
       </c>
@@ -7354,7 +7416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44627</v>
       </c>
@@ -7377,7 +7439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44627</v>
       </c>
@@ -7400,7 +7462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44074</v>
       </c>
@@ -7424,7 +7486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44627</v>
       </c>
@@ -7447,7 +7509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44628</v>
       </c>
@@ -7470,7 +7532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44655</v>
       </c>
@@ -7493,7 +7555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44783</v>
       </c>
@@ -7516,7 +7578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44783</v>
       </c>
@@ -7547,96 +7609,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24FBA74-073E-46F2-A677-303D1306A835}">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>44116</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
-        <v>44627.724999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>44119</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3">
-        <v>500</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
-        <v>44627.724999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>44551</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4">
-        <v>-7000</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
-        <v>44627.724999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940DB676-0691-4D6D-967D-ED592843676B}">
   <dimension ref="A1:L6"/>
   <sheetViews>
@@ -7644,18 +7616,18 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="51.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -7693,7 +7665,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -7732,7 +7704,7 @@
         <v>44628.725694444445</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -7771,7 +7743,7 @@
         <v>44628.725694444445</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -7810,7 +7782,7 @@
         <v>44628.725694444445</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -7849,7 +7821,7 @@
         <v>44628.725694444445</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -7893,26 +7865,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E0FC90-FDA7-4CD4-B785-694A9C9D6F8B}">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7938,7 +7910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44631</v>
       </c>
@@ -7964,7 +7936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44631</v>
       </c>
@@ -7990,7 +7962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44631</v>
       </c>
@@ -8016,7 +7988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44631</v>
       </c>
@@ -8042,7 +8014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44631</v>
       </c>
@@ -8068,7 +8040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44631</v>
       </c>
@@ -8094,7 +8066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44631</v>
       </c>
@@ -8120,7 +8092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44631</v>
       </c>
@@ -8146,7 +8118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44631</v>
       </c>
@@ -8172,7 +8144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44631</v>
       </c>
@@ -8198,7 +8170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44631</v>
       </c>
@@ -8224,7 +8196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44631</v>
       </c>
@@ -8250,7 +8222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44631</v>
       </c>
@@ -8276,7 +8248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44631</v>
       </c>
@@ -8302,7 +8274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44631</v>
       </c>
@@ -8328,7 +8300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44631</v>
       </c>
@@ -8354,7 +8326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44631</v>
       </c>
@@ -8380,7 +8352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44631</v>
       </c>
@@ -8406,7 +8378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44631</v>
       </c>
@@ -8432,7 +8404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44631</v>
       </c>
@@ -8458,7 +8430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44631</v>
       </c>
@@ -8484,7 +8456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44631</v>
       </c>
@@ -8510,7 +8482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44631</v>
       </c>
@@ -8536,7 +8508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44631</v>
       </c>
@@ -8562,7 +8534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44631</v>
       </c>
@@ -8588,7 +8560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44631</v>
       </c>
@@ -8614,7 +8586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44631</v>
       </c>
@@ -8640,7 +8612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44631</v>
       </c>
@@ -8666,7 +8638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44631</v>
       </c>
@@ -8692,7 +8664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44631</v>
       </c>
@@ -8718,7 +8690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44631</v>
       </c>
@@ -8744,7 +8716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44631</v>
       </c>
@@ -8770,7 +8742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44631</v>
       </c>
@@ -8796,7 +8768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44655</v>
       </c>
@@ -8822,7 +8794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44783</v>
       </c>
@@ -8848,7 +8820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44783</v>
       </c>
@@ -8885,37 +8857,393 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE640F6-67C2-41C5-A6DC-CD9104FE1D7C}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="str">
+        <f>E2&amp;" "&amp;C2</f>
+        <v>TFSA Ke</v>
+      </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44013</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B7" si="0">E3&amp;" "&amp;C3</f>
+        <v>RRSP Ke</v>
+      </c>
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>44752</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>LIRA Ke</v>
+      </c>
+      <c r="C4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>44621</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>TFSA Saving Ke</v>
+      </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44713</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>TFSA Tong</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>44788</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>TFSA Saving Tong</v>
+      </c>
+      <c r="C7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>44713</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19D8F81-04A5-4D1F-90EE-02C5BAFD5B03}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24FBA74-073E-46F2-A677-303D1306A835}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G3:G4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
         <v>95</v>
       </c>
       <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12">
+        <v>44627.724999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44119</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3">
+        <v>500</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12">
+        <v>44627.724999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44551</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4">
+        <v>-7000</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>44627.724999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44791</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5">
+        <v>20000</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12">
+        <v>44793.875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44791</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <v>44794.923611111109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19D8F81-04A5-4D1F-90EE-02C5BAFD5B03}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
       </c>
       <c r="E1" t="s">
         <v>93</v>
@@ -8927,18 +9255,18 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44637</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E2" s="18">
         <v>139895.32999999999</v>
@@ -8950,41 +9278,41 @@
         <v>44784.838888888888</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44784</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E3" s="18">
         <v>134823</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="12">
         <v>44784.838888888888</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44586</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E4" s="18">
         <v>50000</v>
@@ -8996,18 +9324,18 @@
         <v>44784.838888888888</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44616</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E5" s="18">
         <v>15000</v>
@@ -9019,18 +9347,18 @@
         <v>44784.838888888888</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44742</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E6" s="18">
         <v>20000</v>
@@ -9042,35 +9370,227 @@
         <v>44784.838888888888</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44784</v>
       </c>
       <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="E7" s="18">
         <v>85406</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="12">
         <v>44784.838888888888</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44785</v>
+      </c>
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8">
+        <v>86291.04</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="19">
+        <v>44785.741157407407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44785</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9">
+        <v>135929.89000000001</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="19">
+        <v>44785.743425925924</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44788</v>
+      </c>
+      <c r="B10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10">
+        <v>137980.89000000001</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19">
+        <v>44788.905960648146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44788</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11">
+        <v>90309.41</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="19">
+        <v>44788.908159722225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44789</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12">
+        <v>90235.98</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="19">
+        <v>44789.871087962965</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44789</v>
+      </c>
+      <c r="B13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13">
+        <v>137506.89000000001</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="19">
+        <v>44789.872314814813</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44790</v>
+      </c>
+      <c r="B14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14">
+        <v>89877.63</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="19">
+        <v>44791.728495370371</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44790</v>
+      </c>
+      <c r="B15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15">
+        <v>136786.14000000001</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="19">
+        <v>44791.729456018518</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{DB11C3E3-B056-422F-AAFC-F6CF592652EC}">
-      <formula1>"LIRA Ke, RRSP Ke, RRSP Tong, TFSA Ke, TFSA Tong"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB11C3E3-B056-422F-AAFC-F6CF592652EC}">
+          <x14:formula1>
+            <xm:f>MyBrokerAccounts!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B15</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>